<commit_message>
Update Sig. upregulated and downregulated proteins.xlsx
</commit_message>
<xml_diff>
--- a/LA of proteome data/1st proteome LA results/Sig. upregulated and downregulated proteins.xlsx
+++ b/LA of proteome data/1st proteome LA results/Sig. upregulated and downregulated proteins.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabde\OneDrive\Documents\UM documents\BMS Year 3\Internship + Thesis\Sabrina_BMS_Bachelor-Internship\R analysis of proteome data\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/34420f5773a88cdb/Documents/UM documents/BMS Year 3/Internship ^M Thesis/Sabrina_BMS_Bachelor-Internship/LA of proteome data/1st proteome LA results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98EB2694-B03F-4617-AB13-8985B51D72F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{98EB2694-B03F-4617-AB13-8985B51D72F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A2716557-3E0C-4B88-A64C-A847FB8BAC41}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="-140" yWindow="0" windowWidth="10510" windowHeight="560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
   <si>
     <t>New Identifier</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t xml:space="preserve">10 upregulated and 15 downregulated </t>
+  </si>
+  <si>
+    <t>up/down regulated using cut off of +/-1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 downregulated </t>
   </si>
 </sst>
 </file>
@@ -485,21 +491,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.7265625" style="5"/>
-    <col min="6" max="6" width="17.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -518,11 +525,12 @@
       <c r="F1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="6"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -542,7 +550,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -562,7 +570,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -582,7 +590,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -602,7 +610,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -622,7 +630,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -642,7 +650,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -662,7 +670,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
@@ -682,7 +690,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
@@ -702,7 +710,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -722,7 +730,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
@@ -742,7 +750,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
@@ -762,7 +770,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>16</v>
       </c>
@@ -782,7 +790,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
@@ -802,7 +810,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
@@ -822,7 +830,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
@@ -842,7 +850,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
@@ -862,7 +870,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
@@ -882,7 +890,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>22</v>
       </c>
@@ -902,7 +910,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>23</v>
       </c>
@@ -922,7 +930,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>24</v>
       </c>
@@ -942,7 +950,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>25</v>
       </c>
@@ -961,8 +969,11 @@
       <c r="F23" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>26</v>
       </c>
@@ -982,7 +993,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>27</v>
       </c>
@@ -1002,7 +1013,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>28</v>
       </c>
@@ -1020,6 +1031,14 @@
       </c>
       <c r="F26" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F27" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G27" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>